<commit_message>
Atualizando crachas de sobre.html
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de risco.xlsx
+++ b/Documentação/Planilha de risco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bandtec\PI Fase2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Ninth-Group\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -152,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,27 +167,22 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF57140F"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Book Antiqua"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF57140F"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Book Antiqua"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF57140F"/>
-      <name val="Book Antiqua"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Book Antiqua"/>
     </font>
   </fonts>
   <fills count="4">
@@ -199,18 +194,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF9768D1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -219,176 +214,215 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF25064C"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF25064C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF25064C"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </right>
       <top style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </top>
       <bottom style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF25064C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF25064C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF25064C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF25064C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF25064C"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF25064C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF25064C"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </right>
       <top style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </left>
       <right style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </right>
       <top style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="3"/>
+        <color rgb="FF25064C"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF25064C"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF25064C"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF25064C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF25064C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF25064C"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF25064C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF25064C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF25064C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF25064C"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF25064C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF25064C"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF25064C"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,27 +441,29 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Book Antiqua"/>
         <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FF9768D1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="3"/>
+        <left style="thick">
+          <color rgb="FF25064C"/>
         </left>
-        <right/>
+        <right style="thick">
+          <color rgb="FF25064C"/>
+        </right>
         <top style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </bottom>
       </border>
     </dxf>
@@ -455,18 +491,144 @@
       </fill>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="3"/>
+        <left style="thick">
+          <color rgb="FF25064C"/>
         </left>
         <right style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </right>
         <top style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Book Antiqua"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF25064C"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF25064C"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Book Antiqua"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF25064C"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF25064C"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF25064C"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Book Antiqua"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF25064C"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF25064C"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF25064C"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF25064C"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -493,17 +655,25 @@
         </patternFill>
       </fill>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FF25064C"/>
+        </right>
         <top style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </bottom>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -529,19 +699,25 @@
         </patternFill>
       </fill>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </left>
         <right style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </right>
         <top style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </bottom>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -567,115 +743,54 @@
         </patternFill>
       </fill>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </left>
         <right style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </right>
         <top style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thin">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF25064C"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF25064C"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF25064C"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF25064C"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Book Antiqua"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF57140F"/>
-        <name val="Book Antiqua"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </left>
         <right style="thick">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </right>
         <top style="thick">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </top>
         <bottom style="thick">
-          <color theme="3"/>
+          <color rgb="FF25064C"/>
         </bottom>
       </border>
     </dxf>
@@ -703,51 +818,12 @@
       </fill>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF57140F"/>
-        <name val="Book Antiqua"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9768D1"/>
+      <color rgb="FF25064C"/>
       <color rgb="FFF2F2F2"/>
       <color rgb="FF57140F"/>
     </mruColors>
@@ -764,18 +840,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:H19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:H19" totalsRowShown="0" headerRowDxfId="2" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
   <autoFilter ref="B4:H19"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Código" dataDxfId="6"/>
-    <tableColumn id="2" name="Descrição do Risco" dataDxfId="5"/>
-    <tableColumn id="3" name="Probabilidade" dataDxfId="4"/>
-    <tableColumn id="4" name="Impacto" dataDxfId="3"/>
-    <tableColumn id="5" name="Fator de Risco" dataDxfId="2">
+    <tableColumn id="1" name="Código" dataDxfId="0"/>
+    <tableColumn id="2" name="Descrição do Risco" dataDxfId="1"/>
+    <tableColumn id="3" name="Probabilidade" dataDxfId="7"/>
+    <tableColumn id="4" name="Impacto" dataDxfId="6"/>
+    <tableColumn id="5" name="Fator de Risco" dataDxfId="5">
       <calculatedColumnFormula>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Ação" dataDxfId="1"/>
-    <tableColumn id="7" name="Como?" dataDxfId="0"/>
+    <tableColumn id="6" name="Ação" dataDxfId="4"/>
+    <tableColumn id="7" name="Como?" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,7 +1123,7 @@
   <dimension ref="A1:AD38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B4" sqref="B4:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1162,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1099,27 +1175,27 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="1"/>
@@ -1128,26 +1204,26 @@
     </row>
     <row r="5" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="5">
+      <c r="B5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="1"/>
@@ -1156,26 +1232,26 @@
     </row>
     <row r="6" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="5">
+      <c r="B6" s="13">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="1"/>
@@ -1184,26 +1260,26 @@
     </row>
     <row r="7" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="5">
+      <c r="B7" s="13">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>6</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="1"/>
@@ -1212,26 +1288,26 @@
     </row>
     <row r="8" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="5">
+      <c r="B8" s="13">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="1"/>
@@ -1240,26 +1316,26 @@
     </row>
     <row r="9" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5">
+      <c r="B9" s="13">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>4</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="1"/>
@@ -1268,26 +1344,26 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="5">
+      <c r="B10" s="13">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
         <v>2</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>2</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="I10" s="1"/>
@@ -1296,26 +1372,26 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="5">
+      <c r="B11" s="13">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>3</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>3</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="1"/>
@@ -1324,26 +1400,26 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="5">
+      <c r="B12" s="13">
         <v>8</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>6</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I12" s="1"/>
@@ -1352,26 +1428,26 @@
     </row>
     <row r="13" spans="1:11" ht="33" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="5">
+      <c r="B13" s="13">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>1</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I13" s="1"/>
@@ -1380,26 +1456,26 @@
     </row>
     <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="5">
+      <c r="B14" s="13">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="2">
         <v>3</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>3</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="1"/>
@@ -1408,26 +1484,26 @@
     </row>
     <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="5">
+      <c r="B15" s="13">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="2">
         <v>3</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>6</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I15" s="1"/>
@@ -1436,26 +1512,26 @@
     </row>
     <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="9">
+      <c r="B16" s="13">
         <v>12</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="2">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>6</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I16" s="1"/>
@@ -1464,26 +1540,26 @@
     </row>
     <row r="17" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="5">
+      <c r="B17" s="13">
         <v>13</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="5">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>4</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I17" s="1"/>
@@ -1492,26 +1568,26 @@
     </row>
     <row r="18" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>14</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="5">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>4</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I18" s="1"/>
@@ -1537,28 +1613,28 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" ht="33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="14">
         <v>15</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="7">
         <f>PRODUCT(Tabela1[[#This Row],[Probabilidade]],Tabela1[[#This Row],[Impacto]])</f>
         <v>2</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="1"/>
@@ -1584,7 +1660,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>